<commit_message>
fix 45 ammo and mag weights
</commit_message>
<xml_diff>
--- a/changes/45-ammo.xlsx
+++ b/changes/45-ammo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lingl\Documents\deadline-balancing\changes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93A5404-4BE4-4AC3-99E8-6FBF37B77BE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581EA817-4073-4B8D-BE62-021AA94A5D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="9mm-ammo" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>new</t>
   </si>
@@ -156,6 +156,30 @@
   </si>
   <si>
     <t>fmj</t>
+  </si>
+  <si>
+    <t>45acp_speer_golddot_230gr_bjhp</t>
+  </si>
+  <si>
+    <t>.45 ACP Speer Gold Dot 230gr BJHP</t>
+  </si>
+  <si>
+    <t>45acp_ammoinc_230gr_subsonic_tmj</t>
+  </si>
+  <si>
+    <t>.45 ACP Ammo Inc. 230gr Subsonic TMJ</t>
+  </si>
+  <si>
+    <t>45acp_winchester_service_grade_230gr_fmj</t>
+  </si>
+  <si>
+    <t>.45 ACP Winchester Service Grade 230gr FMJ</t>
+  </si>
+  <si>
+    <t>45acp_supernova_225gr_red_tracer</t>
+  </si>
+  <si>
+    <t>.45 ACP Supernova 225gr Red Tracer</t>
   </si>
 </sst>
 </file>
@@ -646,9 +670,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -746,9 +769,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -786,7 +809,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -892,7 +915,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1034,7 +1057,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1045,12 +1068,13 @@
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="1" max="1" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" customWidth="1"/>
     <col min="3" max="14" width="6.7109375" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
     <col min="16" max="23" width="6.7109375" customWidth="1"/>
@@ -1060,22 +1084,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
       <c r="T1" t="s">
         <v>27</v>
       </c>
@@ -1084,46 +1095,46 @@
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" t="s">
         <v>3</v>
       </c>
       <c r="P2" t="s">
@@ -1158,38 +1169,38 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.1</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>-2</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>-2</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2">
         <v>0.1</v>
       </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
         <v>-50</v>
       </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2">
         <v>1200</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3">
         <f>C3-D3*20-E3*0.8-F3*0.6-H3*5+(W3-22)*1+P3/300+S3*2</f>
         <v>17.639999999999997</v>
       </c>
@@ -1199,7 +1210,7 @@
       <c r="Q3">
         <v>20</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="1">
         <v>0.5</v>
       </c>
       <c r="S3">
@@ -1229,34 +1240,34 @@
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>-0.5</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.1</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2">
         <v>0.1</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2">
         <v>1200</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4">
         <f t="shared" ref="N4:N7" si="0">C4-D4*20-E4*0.8-F4*0.6-H4*5+(W4-22)*1+P4/300+S4*2</f>
         <v>21.5</v>
       </c>
@@ -1266,7 +1277,7 @@
       <c r="Q4">
         <v>30</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="1">
         <v>0.5</v>
       </c>
       <c r="S4">
@@ -1296,36 +1307,36 @@
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
         <v>0.1</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2">
         <v>-2</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2">
         <v>0.1</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
         <v>-20</v>
       </c>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3">
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2">
         <v>1500</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5">
         <f t="shared" si="0"/>
         <v>18.479999999999997</v>
       </c>
@@ -1335,7 +1346,7 @@
       <c r="Q5">
         <v>50</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="1">
         <v>0.5</v>
       </c>
       <c r="S5">
@@ -1365,30 +1376,30 @@
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
         <v>0.1</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="1">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="0"/>
         <v>17.866666666666664</v>
       </c>
@@ -1398,7 +1409,7 @@
       <c r="Q6">
         <v>50</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="1">
         <v>0.5</v>
       </c>
       <c r="S6">
@@ -1428,34 +1439,34 @@
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="3">
-        <v>0</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
         <v>0.1</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
         <v>0.1</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3">
+      <c r="I7" s="2"/>
+      <c r="J7" s="2">
         <v>-50</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2">
         <v>1000</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7">
         <f t="shared" si="0"/>
         <v>26.079999999999995</v>
       </c>
@@ -1465,7 +1476,7 @@
       <c r="Q7">
         <v>30</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" s="1">
         <v>0.6</v>
       </c>
       <c r="S7">
@@ -1495,21 +1506,7 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="R8" s="2"/>
+      <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
@@ -1517,42 +1514,40 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" t="s">
         <v>3</v>
       </c>
       <c r="P10" t="s">
@@ -1578,42 +1573,42 @@
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="3">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2">
         <v>1</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
         <v>0.1</v>
       </c>
-      <c r="E11" s="3">
-        <v>0</v>
-      </c>
-      <c r="F11" s="3">
-        <v>1</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>0.14000000000000001</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>100</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2">
         <v>1200</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11">
         <f>C11-D11*20-E11*0.8-F11*0.6-H11*5+(W11-22)*1+P11/300+S11*2</f>
-        <v>18.953333333333337</v>
+        <v>20.953333333333333</v>
       </c>
       <c r="P11">
         <v>1000</v>
@@ -1621,7 +1616,7 @@
       <c r="Q11">
         <v>50</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="1">
         <v>0.4</v>
       </c>
       <c r="S11">
@@ -1645,42 +1640,42 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="3">
+      <c r="A12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="2">
         <v>2</v>
       </c>
-      <c r="D12" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
         <v>-2</v>
       </c>
-      <c r="F12" s="3">
-        <v>0</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3">
+      <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
         <v>-0.13</v>
       </c>
-      <c r="J12" s="3">
-        <v>0</v>
-      </c>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3">
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2">
         <v>1200</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12">
         <f t="shared" ref="N12:N15" si="3">C12-D12*20-E12*0.8-F12*0.6-H12*5+(W12-22)*1+P12/300+S12*2</f>
-        <v>19.46</v>
+        <v>21.46</v>
       </c>
       <c r="P12">
         <v>900</v>
@@ -1688,7 +1683,7 @@
       <c r="Q12">
         <v>50</v>
       </c>
-      <c r="R12" s="2">
+      <c r="R12" s="1">
         <v>0.4</v>
       </c>
       <c r="S12">
@@ -1712,42 +1707,42 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0</v>
-      </c>
-      <c r="D13" s="3">
+      <c r="A13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2">
         <v>0.1</v>
       </c>
-      <c r="E13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="3">
-        <v>-1</v>
-      </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>0.06</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <v>80</v>
       </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3">
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2">
         <v>1500</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N13">
         <f t="shared" si="3"/>
-        <v>19.573333333333338</v>
+        <v>21.573333333333338</v>
       </c>
       <c r="P13">
         <v>980</v>
@@ -1755,7 +1750,7 @@
       <c r="Q13">
         <v>50</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13" s="1">
         <v>0.4</v>
       </c>
       <c r="S13">
@@ -1779,42 +1774,42 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="3">
-        <v>0</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="E14" s="3">
-        <v>0</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3">
-        <v>0</v>
-      </c>
-      <c r="I14" s="3">
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
         <v>0.03</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>80</v>
       </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2">
+        <v>0</v>
+      </c>
+      <c r="N14">
         <f t="shared" si="3"/>
-        <v>18.303333333333338</v>
+        <v>20.303333333333338</v>
       </c>
       <c r="P14">
         <v>980</v>
@@ -1822,7 +1817,7 @@
       <c r="Q14">
         <v>50</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14" s="1">
         <v>0.4</v>
       </c>
       <c r="S14">
@@ -1846,42 +1841,42 @@
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="3">
+      <c r="A15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="2">
         <v>-1</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2">
         <v>0.1</v>
       </c>
-      <c r="E15" s="3">
-        <v>0</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <v>-0.12</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="2">
         <v>170</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3">
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2">
         <v>1000</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15">
         <f t="shared" si="3"/>
-        <v>19.213333333333335</v>
+        <v>21.213333333333335</v>
       </c>
       <c r="P15">
         <v>1070</v>
@@ -1889,7 +1884,7 @@
       <c r="Q15">
         <v>60</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="1">
         <v>0.5</v>
       </c>
       <c r="S15">
@@ -1913,44 +1908,32 @@
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="R16" s="2"/>
+      <c r="R16" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C16:D16 G16:U16 O15:P15 R15:S15">
-    <cfRule type="expression" dxfId="4" priority="1">
-      <formula>C15&lt;&gt;C7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O13:P13 R13:S13">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>O13&lt;&gt;O4</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O11:P11 R11:T11 T12:T15 N11:N15">
-    <cfRule type="expression" dxfId="2" priority="4">
+  <conditionalFormatting sqref="O11:P11 R11:T11 N11:N15 T12:T15">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>N11&lt;&gt;N6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12:P12 R12:S12">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>O12&lt;&gt;O5</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O13:P13 R13:S13">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>O13&lt;&gt;O4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="O14:P14 R14:S14">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>O14&lt;&gt;O3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O15:P15 R15:S15 C16:D16 G16:U16">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>C15&lt;&gt;C7</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>